<commit_message>
updated game class, player class and contribution sheet
</commit_message>
<xml_diff>
--- a/groupUpdateTemplate.xlsx
+++ b/groupUpdateTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\Uni\Year 2\APT\assign2\apt-Group-T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D55393-AC2A-49F9-B062-B26CCFD73883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B804D79-B5B0-4BB5-98BF-35951BCC5401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>Assignment 2 | Weekly Update Tracking Sheet</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Game class, player class (place and replace outline), moved print board to game class, added player hands and added player scores to board layout, began working on tracking turn order.</t>
   </si>
 </sst>
 </file>
@@ -1849,7 +1852,7 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2563,7 +2566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="7"/>
       <c r="C45" s="12"/>
@@ -2574,7 +2577,9 @@
       <c r="F45" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G45" s="16"/>
+      <c r="G45" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="H45" s="17"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>

</xml_diff>